<commit_message>
quelques modifs de texte et d'intégration concernant les prêts et subventions
</commit_message>
<xml_diff>
--- a/static/files/financement.xlsx
+++ b/static/files/financement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE93286-1141-42B1-992D-E22F986AA161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA52747-56EE-4892-B6B7-8B2B7CF19282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -103,9 +103,6 @@
     <t>indiquer l’ensemble des prêts et subventions.</t>
   </si>
   <si>
-    <t>Autre</t>
-  </si>
-  <si>
     <t>Commune et action logement</t>
   </si>
   <si>
@@ -116,6 +113,15 @@
   </si>
   <si>
     <t>Etat</t>
+  </si>
+  <si>
+    <t>Autre/Subventions</t>
+  </si>
+  <si>
+    <t>sqdfgth</t>
+  </si>
+  <si>
+    <t>suuuub</t>
   </si>
 </sst>
 </file>
@@ -347,23 +353,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -780,7 +786,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -820,12 +826,24 @@
       <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="17"/>
+      <c r="A3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="14">
+        <v>28972</v>
+      </c>
+      <c r="C3" s="15">
+        <v>3</v>
+      </c>
+      <c r="D3" s="16">
+        <v>34000</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -1070,7 +1088,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1106,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="21">
         <v>3</v>
@@ -1106,12 +1124,12 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,7 +1139,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1131,11 +1149,11 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qBPxnFKf6czTrHsTZILOr2KteNUZQGS7Y0GWwiULBQUW1FaCBh1QHoSf+Nvt49WmQ5xh8wujjOhbB+uFBFRxsg==" saltValue="rCR27LIFOeQEvhrf4mKk+w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="twTmi6Rd4fQavULxqJZ3e7rcu7uzEmZnyeESM2YvXe5kicWDvqpc17t2PBPEc9sUGpwS9d1XWWn2H7NEO92iUQ==" saltValue="rqEtg/lYY4Jz7LUBKK/nJg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
quelques modifs de texte et d'intégration concernant les prêts et subventions (#669)
</commit_message>
<xml_diff>
--- a/static/files/financement.xlsx
+++ b/static/files/financement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE93286-1141-42B1-992D-E22F986AA161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA52747-56EE-4892-B6B7-8B2B7CF19282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -103,9 +103,6 @@
     <t>indiquer l’ensemble des prêts et subventions.</t>
   </si>
   <si>
-    <t>Autre</t>
-  </si>
-  <si>
     <t>Commune et action logement</t>
   </si>
   <si>
@@ -116,6 +113,15 @@
   </si>
   <si>
     <t>Etat</t>
+  </si>
+  <si>
+    <t>Autre/Subventions</t>
+  </si>
+  <si>
+    <t>sqdfgth</t>
+  </si>
+  <si>
+    <t>suuuub</t>
   </si>
 </sst>
 </file>
@@ -347,23 +353,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -780,7 +786,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -820,12 +826,24 @@
       <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="17"/>
+      <c r="A3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="14">
+        <v>28972</v>
+      </c>
+      <c r="C3" s="15">
+        <v>3</v>
+      </c>
+      <c r="D3" s="16">
+        <v>34000</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -1070,7 +1088,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1106,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="21">
         <v>3</v>
@@ -1106,12 +1124,12 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,7 +1139,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1131,11 +1149,11 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qBPxnFKf6czTrHsTZILOr2KteNUZQGS7Y0GWwiULBQUW1FaCBh1QHoSf+Nvt49WmQ5xh8wujjOhbB+uFBFRxsg==" saltValue="rCR27LIFOeQEvhrf4mKk+w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="twTmi6Rd4fQavULxqJZ3e7rcu7uzEmZnyeESM2YvXe5kicWDvqpc17t2PBPEc9sUGpwS9d1XWWn2H7NEO92iUQ==" saltValue="rqEtg/lYY4Jz7LUBKK/nJg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
financement : remove useless line in xlsx template
</commit_message>
<xml_diff>
--- a/static/files/financement.xlsx
+++ b/static/files/financement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA52747-56EE-4892-B6B7-8B2B7CF19282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6605EF-6FC6-BA47-B5BA-6BCF128E8662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="34020" yWindow="4040" windowWidth="27740" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Financements" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -116,12 +116,6 @@
   </si>
   <si>
     <t>Autre/Subventions</t>
-  </si>
-  <si>
-    <t>sqdfgth</t>
-  </si>
-  <si>
-    <t>suuuub</t>
   </si>
 </sst>
 </file>
@@ -487,7 +481,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -786,18 +780,18 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="20.875" customWidth="1"/>
-    <col min="5" max="5" width="30.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.875" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
@@ -817,7 +811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="26"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -825,27 +819,15 @@
       <c r="E2" s="28"/>
       <c r="F2" s="24"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="14">
-        <v>28972</v>
-      </c>
-      <c r="C3" s="15">
-        <v>3</v>
-      </c>
-      <c r="D3" s="16">
-        <v>34000</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
@@ -853,7 +835,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
@@ -861,7 +843,7 @@
       <c r="E5" s="15"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
@@ -869,7 +851,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
@@ -877,7 +859,7 @@
       <c r="E7" s="15"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
@@ -885,7 +867,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -893,7 +875,7 @@
       <c r="E9" s="15"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
@@ -901,7 +883,7 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
@@ -909,7 +891,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
@@ -917,7 +899,7 @@
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
@@ -925,7 +907,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
@@ -933,7 +915,7 @@
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
@@ -941,7 +923,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -949,7 +931,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -957,7 +939,7 @@
       <c r="E17" s="15"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -965,7 +947,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -973,7 +955,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -981,7 +963,7 @@
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
@@ -989,7 +971,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="18"/>
       <c r="C22" s="6"/>
@@ -1031,48 +1013,48 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" s="22" t="s">
         <v>19</v>
       </c>
@@ -1091,12 +1073,12 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1104,7 +1086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -1112,42 +1094,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
financement : remove useless line in xlsx template (#856)
</commit_message>
<xml_diff>
--- a/static/files/financement.xlsx
+++ b/static/files/financement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA52747-56EE-4892-B6B7-8B2B7CF19282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6605EF-6FC6-BA47-B5BA-6BCF128E8662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="34020" yWindow="4040" windowWidth="27740" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Financements" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -116,12 +116,6 @@
   </si>
   <si>
     <t>Autre/Subventions</t>
-  </si>
-  <si>
-    <t>sqdfgth</t>
-  </si>
-  <si>
-    <t>suuuub</t>
   </si>
 </sst>
 </file>
@@ -487,7 +481,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -786,18 +780,18 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="20.875" customWidth="1"/>
-    <col min="5" max="5" width="30.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.875" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
@@ -817,7 +811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="26"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -825,27 +819,15 @@
       <c r="E2" s="28"/>
       <c r="F2" s="24"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="14">
-        <v>28972</v>
-      </c>
-      <c r="C3" s="15">
-        <v>3</v>
-      </c>
-      <c r="D3" s="16">
-        <v>34000</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
@@ -853,7 +835,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
@@ -861,7 +843,7 @@
       <c r="E5" s="15"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
@@ -869,7 +851,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
@@ -877,7 +859,7 @@
       <c r="E7" s="15"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
@@ -885,7 +867,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -893,7 +875,7 @@
       <c r="E9" s="15"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
@@ -901,7 +883,7 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
@@ -909,7 +891,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
@@ -917,7 +899,7 @@
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
@@ -925,7 +907,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
@@ -933,7 +915,7 @@
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
@@ -941,7 +923,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -949,7 +931,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -957,7 +939,7 @@
       <c r="E17" s="15"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -965,7 +947,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -973,7 +955,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -981,7 +963,7 @@
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
@@ -989,7 +971,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="18"/>
       <c r="C22" s="6"/>
@@ -1031,48 +1013,48 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" s="22" t="s">
         <v>19</v>
       </c>
@@ -1091,12 +1073,12 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1104,7 +1086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -1112,42 +1094,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Ajout d'une mention pour les prêts en cours de signature
</commit_message>
<xml_diff>
--- a/static/files/financement.xlsx
+++ b/static/files/financement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBB9BC6-FF7D-2E4D-9B14-C6E0D2C90DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762975EC-3214-904C-AAA5-0B56EA998315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36040" yWindow="520" windowWidth="27740" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1420" yWindow="760" windowWidth="28820" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Financements" sheetId="1" r:id="rId1"/>
@@ -66,10 +66,6 @@
 (en €)</t>
   </si>
   <si>
-    <t>Durée
-(en années)</t>
-  </si>
-  <si>
     <t>Date d'octroi
 (format dd/mm/yyyy)</t>
   </si>
@@ -116,6 +112,25 @@
   </si>
   <si>
     <t>Autre/Subventions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Durée
+(en années)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Si le prêt est en cours de signature, indiquez une durée indicative</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -125,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,6 +178,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -738,7 +762,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,21 +773,21 @@
     <col min="6" max="6" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>5</v>
@@ -987,7 +1011,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1002,7 +1026,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
@@ -1012,7 +1036,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1037,12 +1061,12 @@
         <v>7</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="16">
         <v>3</v>
@@ -1050,22 +1074,22 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1075,17 +1099,17 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout d'une mention pour les prêts en cours de signature (#1823)
</commit_message>
<xml_diff>
--- a/static/files/financement.xlsx
+++ b/static/files/financement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBB9BC6-FF7D-2E4D-9B14-C6E0D2C90DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762975EC-3214-904C-AAA5-0B56EA998315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36040" yWindow="520" windowWidth="27740" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1420" yWindow="760" windowWidth="28820" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Financements" sheetId="1" r:id="rId1"/>
@@ -66,10 +66,6 @@
 (en €)</t>
   </si>
   <si>
-    <t>Durée
-(en années)</t>
-  </si>
-  <si>
     <t>Date d'octroi
 (format dd/mm/yyyy)</t>
   </si>
@@ -116,6 +112,25 @@
   </si>
   <si>
     <t>Autre/Subventions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Durée
+(en années)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Si le prêt est en cours de signature, indiquez une durée indicative</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -125,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,6 +178,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -738,7 +762,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,21 +773,21 @@
     <col min="6" max="6" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>5</v>
@@ -987,7 +1011,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1002,7 +1026,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
@@ -1012,7 +1036,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1037,12 +1061,12 @@
         <v>7</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="16">
         <v>3</v>
@@ -1050,22 +1074,22 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1075,17 +1099,17 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AM-65 Modification Prêteur -> Organisme financeur (#2042)
* ajout de Financeur à la colonne preteur

* renommage organisme financeur

* modif colonne excel

* modification du xlsx

---------

Co-authored-by: adrien.abescat <adrien.abescat@sullly-group.fr>
</commit_message>
<xml_diff>
--- a/static/files/financement.xlsx
+++ b/static/files/financement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projets\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762975EC-3214-904C-AAA5-0B56EA998315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321A531B-BB5A-4F31-8DC0-F9A7D4E8262B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="760" windowWidth="28820" windowHeight="18880" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="28332" yWindow="1008" windowWidth="23040" windowHeight="12120" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Financements" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Attention, en aucun cas vous ne devez modifier l'entête du tableau des prêts, cela casserait l'import des données</t>
   </si>
   <si>
-    <t>Préciser l'identité du préteur si vous avez sélectionné 'Autre'</t>
-  </si>
-  <si>
     <t>EPCI</t>
   </si>
   <si>
@@ -72,10 +69,6 @@
   <si>
     <t>Numéro
 (caractères alphanuméric)</t>
-  </si>
-  <si>
-    <t>Prêteur
-(choisir dans la liste déroulante)</t>
   </si>
   <si>
     <t>CDC pour le foncier</t>
@@ -131,6 +124,13 @@
       </rPr>
       <t>Si le prêt est en cours de signature, indiquez une durée indicative</t>
     </r>
+  </si>
+  <si>
+    <t>Organisme financeur
+(choisir dans la liste déroulante)</t>
+  </si>
+  <si>
+    <t>Préciser l'identité de l'organisme financeur si vous avez sélectionné 'Autre'</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -762,38 +762,38 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.796875" customWidth="1"/>
+    <col min="5" max="5" width="30.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -801,7 +801,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
@@ -809,7 +809,7 @@
       <c r="E3" s="12"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -817,7 +817,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -825,7 +825,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -833,7 +833,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -841,7 +841,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
@@ -849,7 +849,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
@@ -857,7 +857,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -865,7 +865,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
@@ -873,7 +873,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
@@ -881,7 +881,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
@@ -889,7 +889,7 @@
       <c r="E13" s="12"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
@@ -897,7 +897,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -905,7 +905,7 @@
       <c r="E15" s="12"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -913,7 +913,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12"/>
@@ -921,7 +921,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -929,7 +929,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="12"/>
@@ -937,7 +937,7 @@
       <c r="E19" s="12"/>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -945,7 +945,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
@@ -953,7 +953,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="14"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -993,50 +993,50 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1051,65 +1051,65 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>